<commit_message>
Two inputs and outputs
</commit_message>
<xml_diff>
--- a/model/model.xlsx
+++ b/model/model.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tamc/Downloads/calculator-workshop-live/model/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60AA6323-E783-4046-BF31-48A790844D14}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED13395-8851-E649-B3D5-28D24E691FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" xr2:uid="{493D8BAE-2034-9C49-94CA-F188F5026A5F}"/>
   </bookViews>
@@ -16,8 +16,10 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="capacity">Sheet1!$B$2</definedName>
-    <definedName name="output">Sheet1!$B$6</definedName>
+    <definedName name="input.capacity">Sheet1!$B$2</definedName>
+    <definedName name="input.load_factor">Sheet1!$B$3</definedName>
+    <definedName name="output.energy">Sheet1!$B$6</definedName>
+    <definedName name="output.revenue">Sheet1!$B$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>Our wind turbine</t>
   </si>
@@ -61,6 +63,18 @@
   </si>
   <si>
     <t>MWh</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>£/MWh</t>
+  </si>
+  <si>
+    <t>Annual revenue</t>
+  </si>
+  <si>
+    <t>£/yr</t>
   </si>
 </sst>
 </file>
@@ -413,13 +427,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF6208D7-B706-7D40-BC7F-FB6F7ADD75B0}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="181" zoomScaleNormal="181" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -478,6 +495,29 @@
         <v>7</v>
       </c>
     </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <f>B7*output.energy</f>
+        <v>788940</v>
+      </c>
+      <c r="C8" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>